<commit_message>
Nova entrada de dados
</commit_message>
<xml_diff>
--- a/aula/streamlit/data/Calorias Estrogonofe (respostas).xlsx
+++ b/aula/streamlit/data/Calorias Estrogonofe (respostas).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/808ebfd9a0d86213/ICC/Disciplinas/Disc - Python Intermediário/script/aula/streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_15BED5FA0969696746532C05DCB4A5187680F76F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{294766A6-908F-4436-B1FB-EB5EA344E524}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_33AF74FDAC69AB4CF4522C05DCB4A518C60D5810" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89DCE674-98C9-4104-85BB-040568B3C228}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:C16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:C24">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Carimbo de data/hora"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="gramas"/>
@@ -550,11 +550,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -731,14 +731,102 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="10">
+      <c r="A16" s="4">
         <v>45755.58071923611</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="5">
         <v>358</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="6">
         <v>672</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>45755.591476504633</v>
+      </c>
+      <c r="B17" s="8">
+        <v>350</v>
+      </c>
+      <c r="C17" s="9">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>45755.609441886569</v>
+      </c>
+      <c r="B18" s="5">
+        <v>800</v>
+      </c>
+      <c r="C18" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>45755.657248310185</v>
+      </c>
+      <c r="B19" s="8">
+        <v>450</v>
+      </c>
+      <c r="C19" s="9">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>45755.657509606477</v>
+      </c>
+      <c r="B20" s="5">
+        <v>600</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>45755.779672268516</v>
+      </c>
+      <c r="B21" s="8">
+        <v>500</v>
+      </c>
+      <c r="C21" s="9">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>45755.779805428239</v>
+      </c>
+      <c r="B22" s="5">
+        <v>100</v>
+      </c>
+      <c r="C22" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>45755.779920405097</v>
+      </c>
+      <c r="B23" s="8">
+        <v>350</v>
+      </c>
+      <c r="C23" s="9">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>45755.780091770837</v>
+      </c>
+      <c r="B24" s="11">
+        <v>500</v>
+      </c>
+      <c r="C24" s="12">
+        <v>680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>